<commit_message>
feat: add iv surface
</commit_message>
<xml_diff>
--- a/backtest/proj-iv-surface/iv.xlsx
+++ b/backtest/proj-iv-surface/iv.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD4DE20-0BB3-4847-9B6D-A6CD6CD346BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="21795" windowHeight="13875" activeTab="1"/>
+    <workbookView xWindow="28690" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +15,7 @@
   <externalReferences>
     <externalReference r:id="rId4"/>
   </externalReferences>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -29,8 +30,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="237">
   <si>
     <t>到期日</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -751,12 +774,16 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>计算隐波</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="176" formatCode="#,##0.0000"/>
     <numFmt numFmtId="177" formatCode="yyyy\-mm\-dd"/>
@@ -826,8 +853,11 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="Sheet1"/>
       <sheetName val="Sheet2"/>
@@ -846,9 +876,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -886,9 +916,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -923,7 +953,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -958,7 +988,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1131,7 +1161,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E90"/>
   <sheetViews>
@@ -1139,21 +1169,21 @@
       <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.5" customWidth="1"/>
-    <col min="2" max="2" width="20.125" customWidth="1"/>
-    <col min="4" max="4" width="12.625" customWidth="1"/>
-    <col min="5" max="5" width="15.25" customWidth="1"/>
+    <col min="1" max="1" width="16.46484375" customWidth="1"/>
+    <col min="2" max="2" width="20.1328125" customWidth="1"/>
+    <col min="4" max="4" width="12.59765625" customWidth="1"/>
+    <col min="5" max="5" width="15.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1" s="4">
         <v>45700</v>
       </c>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>89</v>
       </c>
@@ -1170,7 +1200,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>91</v>
       </c>
@@ -1191,7 +1221,7 @@
         <v>6.4823000000000004</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -1212,7 +1242,7 @@
         <v>12.298</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -1233,7 +1263,7 @@
         <v>47.462600000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -1254,7 +1284,7 @@
         <v>22.928100000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -1275,7 +1305,7 @@
         <v>7.4886999999999997</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -1296,7 +1326,7 @@
         <v>2.2805</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -1317,7 +1347,7 @@
         <v>52.8292</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
@@ -1338,7 +1368,7 @@
         <v>35.406999999999996</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
@@ -1359,7 +1389,7 @@
         <v>77.385400000000004</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
@@ -1380,7 +1410,7 @@
         <v>565.51819999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -1401,7 +1431,7 @@
         <v>612.58109999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
@@ -1422,7 +1452,7 @@
         <v>969.76969999999994</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
@@ -1443,7 +1473,7 @@
         <v>44.841799999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
@@ -1464,7 +1494,7 @@
         <v>24.121700000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
@@ -1485,7 +1515,7 @@
         <v>320.52339999999998</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
@@ -1506,7 +1536,7 @@
         <v>319.84980000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
@@ -1527,7 +1557,7 @@
         <v>45.317599999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
@@ -1548,7 +1578,7 @@
         <v>30.769500000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
@@ -1569,7 +1599,7 @@
         <v>20.596499999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
@@ -1590,7 +1620,7 @@
         <v>2.0461</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
@@ -1611,7 +1641,7 @@
         <v>12.3719</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
@@ -1632,7 +1662,7 @@
         <v>16.763999999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>24</v>
       </c>
@@ -1653,7 +1683,7 @@
         <v>38.962899999999998</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>25</v>
       </c>
@@ -1674,7 +1704,7 @@
         <v>235.39519999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>26</v>
       </c>
@@ -1695,7 +1725,7 @@
         <v>514.529</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>27</v>
       </c>
@@ -1716,7 +1746,7 @@
         <v>91.750900000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>28</v>
       </c>
@@ -1737,7 +1767,7 @@
         <v>75.489900000000006</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>29</v>
       </c>
@@ -1758,7 +1788,7 @@
         <v>191.67349999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>30</v>
       </c>
@@ -1779,7 +1809,7 @@
         <v>160.90530000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>31</v>
       </c>
@@ -1800,7 +1830,7 @@
         <v>507.40089999999998</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>32</v>
       </c>
@@ -1821,7 +1851,7 @@
         <v>23.9375</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>33</v>
       </c>
@@ -1842,7 +1872,7 @@
         <v>816.83370000000002</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>34</v>
       </c>
@@ -1863,7 +1893,7 @@
         <v>13.6762</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>35</v>
       </c>
@@ -1884,7 +1914,7 @@
         <v>93.763300000000001</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>36</v>
       </c>
@@ -1905,7 +1935,7 @@
         <v>667.19839999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>37</v>
       </c>
@@ -1926,7 +1956,7 @@
         <v>2044.0472</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>38</v>
       </c>
@@ -1947,7 +1977,7 @@
         <v>3611.9078</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>39</v>
       </c>
@@ -1968,7 +1998,7 @@
         <v>610.17899999999997</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>40</v>
       </c>
@@ -1989,7 +2019,7 @@
         <v>35.558399999999999</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>41</v>
       </c>
@@ -2010,7 +2040,7 @@
         <v>6.3784999999999998</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>42</v>
       </c>
@@ -2031,7 +2061,7 @@
         <v>3.2216</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>43</v>
       </c>
@@ -2052,7 +2082,7 @@
         <v>1.0946</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>44</v>
       </c>
@@ -2073,7 +2103,7 @@
         <v>7.0895999999999999</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>45</v>
       </c>
@@ -2094,7 +2124,7 @@
         <v>11.4115</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>46</v>
       </c>
@@ -2115,7 +2145,7 @@
         <v>25.0562</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>47</v>
       </c>
@@ -2136,7 +2166,7 @@
         <v>13.6975</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>48</v>
       </c>
@@ -2157,7 +2187,7 @@
         <v>141.27889999999999</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>49</v>
       </c>
@@ -2178,7 +2208,7 @@
         <v>628.93539999999996</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>50</v>
       </c>
@@ -2199,7 +2229,7 @@
         <v>11846.1913</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>51</v>
       </c>
@@ -2220,7 +2250,7 @@
         <v>36825.517999999996</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>2</v>
       </c>
@@ -2241,7 +2271,7 @@
         <v>10507.7309</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>52</v>
       </c>
@@ -2262,7 +2292,7 @@
         <v>611.00149999999996</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>53</v>
       </c>
@@ -2283,7 +2313,7 @@
         <v>53.297499999999999</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>54</v>
       </c>
@@ -2304,7 +2334,7 @@
         <v>1.0104</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>55</v>
       </c>
@@ -2325,7 +2355,7 @@
         <v>0.91659999999999997</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>56</v>
       </c>
@@ -2346,7 +2376,7 @@
         <v>37.785400000000003</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>57</v>
       </c>
@@ -2367,7 +2397,7 @@
         <v>197.0188</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>58</v>
       </c>
@@ -2388,7 +2418,7 @@
         <v>957.0675</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>59</v>
       </c>
@@ -2409,7 +2439,7 @@
         <v>2019.6799000000001</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>60</v>
       </c>
@@ -2430,7 +2460,7 @@
         <v>1498.9635000000001</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>61</v>
       </c>
@@ -2451,7 +2481,7 @@
         <v>1291.5923</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>62</v>
       </c>
@@ -2472,7 +2502,7 @@
         <v>176.48949999999999</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>63</v>
       </c>
@@ -2493,7 +2523,7 @@
         <v>22.951799999999999</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>64</v>
       </c>
@@ -2514,7 +2544,7 @@
         <v>2.8090999999999999</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>65</v>
       </c>
@@ -2535,7 +2565,7 @@
         <v>33.195</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>66</v>
       </c>
@@ -2556,7 +2586,7 @@
         <v>27.894300000000001</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>67</v>
       </c>
@@ -2577,7 +2607,7 @@
         <v>198.76070000000001</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>68</v>
       </c>
@@ -2598,7 +2628,7 @@
         <v>433.15179999999998</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>69</v>
       </c>
@@ -2619,7 +2649,7 @@
         <v>608.38670000000002</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>70</v>
       </c>
@@ -2640,7 +2670,7 @@
         <v>265.32220000000001</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>71</v>
       </c>
@@ -2661,7 +2691,7 @@
         <v>180.06559999999999</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>72</v>
       </c>
@@ -2682,7 +2712,7 @@
         <v>4.8859000000000004</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>73</v>
       </c>
@@ -2703,7 +2733,7 @@
         <v>19.613</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>74</v>
       </c>
@@ -2724,7 +2754,7 @@
         <v>161.4693</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>75</v>
       </c>
@@ -2745,7 +2775,7 @@
         <v>39.491199999999999</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>76</v>
       </c>
@@ -2766,7 +2796,7 @@
         <v>6.6824000000000003</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>77</v>
       </c>
@@ -2787,7 +2817,7 @@
         <v>2.56</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>78</v>
       </c>
@@ -2808,7 +2838,7 @@
         <v>52.734000000000002</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>79</v>
       </c>
@@ -2829,7 +2859,7 @@
         <v>37.620800000000003</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>80</v>
       </c>
@@ -2850,7 +2880,7 @@
         <v>311.97089999999997</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>81</v>
       </c>
@@ -2871,7 +2901,7 @@
         <v>529.56849999999997</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>82</v>
       </c>
@@ -2892,7 +2922,7 @@
         <v>62.171599999999998</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>83</v>
       </c>
@@ -2913,7 +2943,7 @@
         <v>58.917900000000003</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>84</v>
       </c>
@@ -2934,7 +2964,7 @@
         <v>116.7212</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>85</v>
       </c>
@@ -2955,7 +2985,7 @@
         <v>0.4405</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>86</v>
       </c>
@@ -2976,7 +3006,7 @@
         <v>19.525600000000001</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>87</v>
       </c>
@@ -2997,7 +3027,7 @@
         <v>186.4323</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>88</v>
       </c>
@@ -3026,25 +3056,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:K138"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.125" customWidth="1"/>
-    <col min="8" max="8" width="23.875" customWidth="1"/>
-    <col min="11" max="11" width="20.125" customWidth="1"/>
+    <col min="1" max="1" width="17.46484375" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="11.1328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.1328125" customWidth="1"/>
+    <col min="8" max="8" width="23.86328125" customWidth="1"/>
+    <col min="9" max="9" width="12.19921875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>231</v>
       </c>
@@ -3052,7 +3083,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>230</v>
       </c>
@@ -3061,7 +3092,7 @@
       </c>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>89</v>
       </c>
@@ -3086,8 +3117,11 @@
       <c r="H3" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="I3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>93</v>
       </c>
@@ -3119,8 +3153,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A4,$B$2)</f>
         <v>578</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="I4" cm="1">
+        <f t="array" ref="I4">iv($B$1,$B$2,G4,B4,C4,H4)</f>
+        <v>3.2760158830058385E-13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>94</v>
       </c>
@@ -3152,8 +3190,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A5,$B$2)</f>
         <v>528</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="I5" cm="1">
+        <f t="array" ref="I5">iv($B$1,$B$2,G5,B5,C5,H5)</f>
+        <v>5.4517977044339742E-13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>95</v>
       </c>
@@ -3185,8 +3227,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A6,$B$2)</f>
         <v>478</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="I6" cm="1">
+        <f t="array" ref="I6">iv($B$1,$B$2,G6,B6,C6,H6)</f>
+        <v>5.0496631950301478E-13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>96</v>
       </c>
@@ -3218,8 +3264,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A7,$B$2)</f>
         <v>428</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="I7" cm="1">
+        <f t="array" ref="I7">iv($B$1,$B$2,G7,B7,C7,H7)</f>
+        <v>1.3923922656864336E-12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>97</v>
       </c>
@@ -3251,8 +3301,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A8,$B$2)</f>
         <v>378</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="I8" cm="1">
+        <f t="array" ref="I8">iv($B$1,$B$2,G8,B8,C8,H8)</f>
+        <v>4.4698000479818411E-13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>98</v>
       </c>
@@ -3284,8 +3338,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A9,$B$2)</f>
         <v>328</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="I9" cm="1">
+        <f t="array" ref="I9">iv($B$1,$B$2,G9,B9,C9,H9)</f>
+        <v>4.7300107658900862E-13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>99</v>
       </c>
@@ -3317,8 +3375,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A10,$B$2)</f>
         <v>271</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="I10" cm="1">
+        <f t="array" ref="I10">iv($B$1,$B$2,G10,B10,C10,H10)</f>
+        <v>1.147176987196448E-13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>100</v>
       </c>
@@ -3350,8 +3412,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A11,$B$2)</f>
         <v>228</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="I11" cm="1">
+        <f t="array" ref="I11">iv($B$1,$B$2,G11,B11,C11,H11)</f>
+        <v>1.0915474796878683E-13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>101</v>
       </c>
@@ -3383,8 +3449,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A12,$B$2)</f>
         <v>175</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="I12" cm="1">
+        <f t="array" ref="I12">iv($B$1,$B$2,G12,B12,C12,H12)</f>
+        <v>1.8911888404723833E-12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>102</v>
       </c>
@@ -3416,8 +3486,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A13,$B$2)</f>
         <v>121.5</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="I13" cm="1">
+        <f t="array" ref="I13">iv($B$1,$B$2,G13,B13,C13,H13)</f>
+        <v>8.5910587386611956E-13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>103</v>
       </c>
@@ -3449,8 +3523,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A14,$B$2)</f>
         <v>77.5</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="I14" cm="1">
+        <f t="array" ref="I14">iv($B$1,$B$2,G14,B14,C14,H14)</f>
+        <v>7.6387621190158431E-13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>104</v>
       </c>
@@ -3482,8 +3560,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A15,$B$2)</f>
         <v>35</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="I15" cm="1">
+        <f t="array" ref="I15">iv($B$1,$B$2,G15,B15,C15,H15)</f>
+        <v>6.7615629248622106E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>105</v>
       </c>
@@ -3515,11 +3597,15 @@
         <f>[1]!thsiFinD("ths_close_price_option",A16,$B$2)</f>
         <v>14</v>
       </c>
+      <c r="I16" cm="1">
+        <f t="array" ref="I16">iv($B$1,$B$2,G16,B16,C16,H16)</f>
+        <v>0.10121812959607057</v>
+      </c>
       <c r="K16" s="5" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>106</v>
       </c>
@@ -3551,8 +3637,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A17,$B$2)</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="I17" cm="1">
+        <f t="array" ref="I17">iv($B$1,$B$2,G17,B17,C17,H17)</f>
+        <v>0.11052920784786618</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>107</v>
       </c>
@@ -3584,8 +3674,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A18,$B$2)</f>
         <v>1.5</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="I18" cm="1">
+        <f t="array" ref="I18">iv($B$1,$B$2,G18,B18,C18,H18)</f>
+        <v>0.12931938535268869</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>108</v>
       </c>
@@ -3617,12 +3711,16 @@
         <f>[1]!thsiFinD("ths_close_price_option",A19,$B$2)</f>
         <v>1</v>
       </c>
+      <c r="I19" cm="1">
+        <f t="array" ref="I19">iv($B$1,$B$2,G19,B19,C19,H19)</f>
+        <v>0.15865637001793814</v>
+      </c>
       <c r="K19" t="str">
-        <f>iv_surface(A3:H138,B1,B2,G3,B3,C3,H3)</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.15">
+        <f>iv_surface(A3:H138,B1,B2,G3,B3,C3,H3,E3)</f>
+        <v>隐含波动率图</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>109</v>
       </c>
@@ -3654,11 +3752,15 @@
         <f>[1]!thsiFinD("ths_close_price_option",A20,$B$2)</f>
         <v>0.5</v>
       </c>
+      <c r="I20" cm="1">
+        <f t="array" ref="I20">iv($B$1,$B$2,G20,B20,C20,H20)</f>
+        <v>0.17661596397460064</v>
+      </c>
       <c r="K20" s="5" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>110</v>
       </c>
@@ -3690,8 +3792,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A21,$B$2)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="I21" cm="1">
+        <f t="array" ref="I21">iv($B$1,$B$2,G21,B21,C21,H21)</f>
+        <v>0.20967583042919821</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>111</v>
       </c>
@@ -3723,8 +3829,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A22,$B$2)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="I22" cm="1">
+        <f t="array" ref="I22">iv($B$1,$B$2,G22,B22,C22,H22)</f>
+        <v>0.2416984896789928</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>112</v>
       </c>
@@ -3756,8 +3866,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A23,$B$2)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="I23" cm="1">
+        <f t="array" ref="I23">iv($B$1,$B$2,G23,B23,C23,H23)</f>
+        <v>0.27282965899413419</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>113</v>
       </c>
@@ -3789,8 +3903,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A24,$B$2)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="I24" cm="1">
+        <f t="array" ref="I24">iv($B$1,$B$2,G24,B24,C24,H24)</f>
+        <v>0.30317356795689882</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>114</v>
       </c>
@@ -3822,8 +3940,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A25,$B$2)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="I25" cm="1">
+        <f t="array" ref="I25">iv($B$1,$B$2,G25,B25,C25,H25)</f>
+        <v>0.33280883506472009</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>115</v>
       </c>
@@ -3855,8 +3977,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A26,$B$2)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="I26" cm="1">
+        <f t="array" ref="I26">iv($B$1,$B$2,G26,B26,C26,H26)</f>
+        <v>0.3617971663787547</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>116</v>
       </c>
@@ -3888,8 +4014,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A27,$B$2)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="I27" cm="1">
+        <f t="array" ref="I27">iv($B$1,$B$2,G27,B27,C27,H27)</f>
+        <v>0.39018851145596317</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>117</v>
       </c>
@@ -3921,8 +4051,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A28,$B$2)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="I28" cm="1">
+        <f t="array" ref="I28">iv($B$1,$B$2,G28,B28,C28,H28)</f>
+        <v>0.41802430939322072</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>118</v>
       </c>
@@ -3954,8 +4088,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A29,$B$2)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="I29" cm="1">
+        <f t="array" ref="I29">iv($B$1,$B$2,G29,B29,C29,H29)</f>
+        <v>0.44533963266035476</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>119</v>
       </c>
@@ -3987,8 +4125,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A30,$B$2)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="I30" cm="1">
+        <f t="array" ref="I30">iv($B$1,$B$2,G30,B30,C30,H30)</f>
+        <v>0.47216465929769363</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>120</v>
       </c>
@@ -4020,8 +4162,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A31,$B$2)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="I31" cm="1">
+        <f t="array" ref="I31">iv($B$1,$B$2,G31,B31,C31,H31)</f>
+        <v>0.49852571724990868</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>121</v>
       </c>
@@ -4053,8 +4199,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A32,$B$2)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I32" cm="1">
+        <f t="array" ref="I32">iv($B$1,$B$2,G32,B32,C32,H32)</f>
+        <v>0.52444604581354992</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>122</v>
       </c>
@@ -4086,8 +4236,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A33,$B$2)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I33" cm="1">
+        <f t="array" ref="I33">iv($B$1,$B$2,G33,B33,C33,H33)</f>
+        <v>0.54994636407152897</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>123</v>
       </c>
@@ -4119,8 +4273,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A34,$B$2)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I34" cm="1">
+        <f t="array" ref="I34">iv($B$1,$B$2,G34,B34,C34,H34)</f>
+        <v>0.57504530401871434</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>124</v>
       </c>
@@ -4152,8 +4310,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A35,$B$2)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I35" cm="1">
+        <f t="array" ref="I35">iv($B$1,$B$2,G35,B35,C35,H35)</f>
+        <v>0.59975974657022413</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>125</v>
       </c>
@@ -4185,8 +4347,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A36,$B$2)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I36" cm="1">
+        <f t="array" ref="I36">iv($B$1,$B$2,G36,B36,C36,H36)</f>
+        <v>0.62410508640659268</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>126</v>
       </c>
@@ -4218,8 +4384,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A37,$B$2)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I37" cm="1">
+        <f t="array" ref="I37">iv($B$1,$B$2,G37,B37,C37,H37)</f>
+        <v>0.67174383560113204</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>127</v>
       </c>
@@ -4251,8 +4421,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A38,$B$2)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I38" cm="1">
+        <f t="array" ref="I38">iv($B$1,$B$2,G38,B38,C38,H38)</f>
+        <v>0.71806209472828275</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>128</v>
       </c>
@@ -4284,8 +4458,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A39,$B$2)</f>
         <v>607</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I39" cm="1">
+        <f t="array" ref="I39">iv($B$1,$B$2,G39,B39,C39,H39)</f>
+        <v>8.5424821105368853E-13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>129</v>
       </c>
@@ -4317,8 +4495,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A40,$B$2)</f>
         <v>557</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I40" cm="1">
+        <f t="array" ref="I40">iv($B$1,$B$2,G40,B40,C40,H40)</f>
+        <v>6.7502439239686883E-13</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>130</v>
       </c>
@@ -4350,8 +4532,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A41,$B$2)</f>
         <v>507</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I41" cm="1">
+        <f t="array" ref="I41">iv($B$1,$B$2,G41,B41,C41,H41)</f>
+        <v>1.5620895775387474E-13</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>131</v>
       </c>
@@ -4383,8 +4569,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A42,$B$2)</f>
         <v>457</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I42" cm="1">
+        <f t="array" ref="I42">iv($B$1,$B$2,G42,B42,C42,H42)</f>
+        <v>4.4362981787573946E-13</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>132</v>
       </c>
@@ -4416,8 +4606,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A43,$B$2)</f>
         <v>407.5</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I43" cm="1">
+        <f t="array" ref="I43">iv($B$1,$B$2,G43,B43,C43,H43)</f>
+        <v>2.8536592640719184E-13</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>133</v>
       </c>
@@ -4449,8 +4643,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A44,$B$2)</f>
         <v>359</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I44" cm="1">
+        <f t="array" ref="I44">iv($B$1,$B$2,G44,B44,C44,H44)</f>
+        <v>2.3834545951604883E-13</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>134</v>
       </c>
@@ -4482,8 +4680,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A45,$B$2)</f>
         <v>311.5</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I45" cm="1">
+        <f t="array" ref="I45">iv($B$1,$B$2,G45,B45,C45,H45)</f>
+        <v>0.1048047791555686</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>135</v>
       </c>
@@ -4515,8 +4717,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A46,$B$2)</f>
         <v>265.5</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I46" cm="1">
+        <f t="array" ref="I46">iv($B$1,$B$2,G46,B46,C46,H46)</f>
+        <v>0.11196818742559987</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>136</v>
       </c>
@@ -4548,8 +4754,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A47,$B$2)</f>
         <v>222.5</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I47" cm="1">
+        <f t="array" ref="I47">iv($B$1,$B$2,G47,B47,C47,H47)</f>
+        <v>0.11731171492932878</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>137</v>
       </c>
@@ -4581,8 +4791,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A48,$B$2)</f>
         <v>169.5</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I48" cm="1">
+        <f t="array" ref="I48">iv($B$1,$B$2,G48,B48,C48,H48)</f>
+        <v>8.8780828256757482E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>138</v>
       </c>
@@ -4614,8 +4828,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A49,$B$2)</f>
         <v>133</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I49" cm="1">
+        <f t="array" ref="I49">iv($B$1,$B$2,G49,B49,C49,H49)</f>
+        <v>9.7283383371601792E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>139</v>
       </c>
@@ -4647,8 +4865,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A50,$B$2)</f>
         <v>97</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I50" cm="1">
+        <f t="array" ref="I50">iv($B$1,$B$2,G50,B50,C50,H50)</f>
+        <v>9.5071990852921742E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>140</v>
       </c>
@@ -4680,8 +4902,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A51,$B$2)</f>
         <v>71.5</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I51" cm="1">
+        <f t="array" ref="I51">iv($B$1,$B$2,G51,B51,C51,H51)</f>
+        <v>0.10026218712263377</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>141</v>
       </c>
@@ -4713,8 +4939,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A52,$B$2)</f>
         <v>52</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I52" cm="1">
+        <f t="array" ref="I52">iv($B$1,$B$2,G52,B52,C52,H52)</f>
+        <v>0.10529150828207257</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>142</v>
       </c>
@@ -4746,8 +4976,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A53,$B$2)</f>
         <v>37</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I53" cm="1">
+        <f t="array" ref="I53">iv($B$1,$B$2,G53,B53,C53,H53)</f>
+        <v>0.1093609156155666</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>143</v>
       </c>
@@ -4779,8 +5013,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A54,$B$2)</f>
         <v>26</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I54" cm="1">
+        <f t="array" ref="I54">iv($B$1,$B$2,G54,B54,C54,H54)</f>
+        <v>0.11321899589718537</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>144</v>
       </c>
@@ -4812,8 +5050,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A55,$B$2)</f>
         <v>20.5</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I55" cm="1">
+        <f t="array" ref="I55">iv($B$1,$B$2,G55,B55,C55,H55)</f>
+        <v>0.12238081146741876</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>145</v>
       </c>
@@ -4845,8 +5087,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A56,$B$2)</f>
         <v>14.5</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I56" cm="1">
+        <f t="array" ref="I56">iv($B$1,$B$2,G56,B56,C56,H56)</f>
+        <v>0.12603871627184129</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>146</v>
       </c>
@@ -4878,8 +5124,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A57,$B$2)</f>
         <v>11</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I57" cm="1">
+        <f t="array" ref="I57">iv($B$1,$B$2,G57,B57,C57,H57)</f>
+        <v>0.13219214100499194</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>147</v>
       </c>
@@ -4911,8 +5161,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A58,$B$2)</f>
         <v>9.5</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I58" cm="1">
+        <f t="array" ref="I58">iv($B$1,$B$2,G58,B58,C58,H58)</f>
+        <v>0.14228716160554675</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>148</v>
       </c>
@@ -4944,8 +5198,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A59,$B$2)</f>
         <v>8.5</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I59" cm="1">
+        <f t="array" ref="I59">iv($B$1,$B$2,G59,B59,C59,H59)</f>
+        <v>0.15283410570012887</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>149</v>
       </c>
@@ -4977,8 +5235,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A60,$B$2)</f>
         <v>6</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I60" cm="1">
+        <f t="array" ref="I60">iv($B$1,$B$2,G60,B60,C60,H60)</f>
+        <v>0.15468702477139537</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>150</v>
       </c>
@@ -5010,8 +5272,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A61,$B$2)</f>
         <v>5.5</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I61" cm="1">
+        <f t="array" ref="I61">iv($B$1,$B$2,G61,B61,C61,H61)</f>
+        <v>0.16470559880555927</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>151</v>
       </c>
@@ -5043,8 +5309,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A62,$B$2)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I62" cm="1">
+        <f t="array" ref="I62">iv($B$1,$B$2,G62,B62,C62,H62)</f>
+        <v>0.12373977062971508</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>152</v>
       </c>
@@ -5076,8 +5346,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A63,$B$2)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I63" cm="1">
+        <f t="array" ref="I63">iv($B$1,$B$2,G63,B63,C63,H63)</f>
+        <v>0.13306684436351382</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>153</v>
       </c>
@@ -5109,8 +5383,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A64,$B$2)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I64" cm="1">
+        <f t="array" ref="I64">iv($B$1,$B$2,G64,B64,C64,H64)</f>
+        <v>0.14221559610306653</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>154</v>
       </c>
@@ -5142,8 +5420,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A65,$B$2)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I65" cm="1">
+        <f t="array" ref="I65">iv($B$1,$B$2,G65,B65,C65,H65)</f>
+        <v>0.15119688173761064</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>155</v>
       </c>
@@ -5175,8 +5457,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A66,$B$2)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I66" cm="1">
+        <f t="array" ref="I66">iv($B$1,$B$2,G66,B66,C66,H66)</f>
+        <v>0.1600200969165462</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>156</v>
       </c>
@@ -5208,8 +5494,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A67,$B$2)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I67" cm="1">
+        <f t="array" ref="I67">iv($B$1,$B$2,G67,B67,C67,H67)</f>
+        <v>0.16869347897584303</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>157</v>
       </c>
@@ -5241,8 +5531,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A68,$B$2)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I68" cm="1">
+        <f t="array" ref="I68">iv($B$1,$B$2,G68,B68,C68,H68)</f>
+        <v>0.17722432932627838</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>158</v>
       </c>
@@ -5274,8 +5568,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A69,$B$2)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I69" cm="1">
+        <f t="array" ref="I69">iv($B$1,$B$2,G69,B69,C69,H69)</f>
+        <v>0.18561918093300289</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>159</v>
       </c>
@@ -5307,8 +5605,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A70,$B$2)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I70" cm="1">
+        <f t="array" ref="I70">iv($B$1,$B$2,G70,B70,C70,H70)</f>
+        <v>0.19388392690939019</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>160</v>
       </c>
@@ -5340,8 +5642,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A71,$B$2)</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I71" cm="1">
+        <f t="array" ref="I71">iv($B$1,$B$2,G71,B71,C71,H71)</f>
+        <v>0.25249861217698055</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>161</v>
       </c>
@@ -5373,8 +5679,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A72,$B$2)</f>
         <v>2.5</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I72" cm="1">
+        <f t="array" ref="I72">iv($B$1,$B$2,G72,B72,C72,H72)</f>
+        <v>0.26445551673684531</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>162</v>
       </c>
@@ -5406,8 +5716,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A73,$B$2)</f>
         <v>611</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I73" cm="1">
+        <f t="array" ref="I73">iv($B$1,$B$2,G73,B73,C73,H73)</f>
+        <v>1.546416009857256E-13</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>163</v>
       </c>
@@ -5439,8 +5753,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A74,$B$2)</f>
         <v>512.5</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I74" cm="1">
+        <f t="array" ref="I74">iv($B$1,$B$2,G74,B74,C74,H74)</f>
+        <v>5.7116401262595083E-14</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>164</v>
       </c>
@@ -5472,8 +5790,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A75,$B$2)</f>
         <v>464.5</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I75" cm="1">
+        <f t="array" ref="I75">iv($B$1,$B$2,G75,B75,C75,H75)</f>
+        <v>9.0493241088900804E-14</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>165</v>
       </c>
@@ -5505,8 +5827,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A76,$B$2)</f>
         <v>417.5</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I76" cm="1">
+        <f t="array" ref="I76">iv($B$1,$B$2,G76,B76,C76,H76)</f>
+        <v>9.6409699055964049E-13</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>166</v>
       </c>
@@ -5538,8 +5864,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A77,$B$2)</f>
         <v>372</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I77" cm="1">
+        <f t="array" ref="I77">iv($B$1,$B$2,G77,B77,C77,H77)</f>
+        <v>7.1096095637413634E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>167</v>
       </c>
@@ -5571,8 +5901,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A78,$B$2)</f>
         <v>328.5</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I78" cm="1">
+        <f t="array" ref="I78">iv($B$1,$B$2,G78,B78,C78,H78)</f>
+        <v>9.7188228656644504E-2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>168</v>
       </c>
@@ -5604,8 +5938,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A79,$B$2)</f>
         <v>286.5</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I79" cm="1">
+        <f t="array" ref="I79">iv($B$1,$B$2,G79,B79,C79,H79)</f>
+        <v>0.10434393762749039</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>169</v>
       </c>
@@ -5637,8 +5975,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A80,$B$2)</f>
         <v>247.5</v>
       </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I80" cm="1">
+        <f t="array" ref="I80">iv($B$1,$B$2,G80,B80,C80,H80)</f>
+        <v>0.10938537161463052</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>170</v>
       </c>
@@ -5670,8 +6012,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A81,$B$2)</f>
         <v>211</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I81" cm="1">
+        <f t="array" ref="I81">iv($B$1,$B$2,G81,B81,C81,H81)</f>
+        <v>0.11227105183465683</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>171</v>
       </c>
@@ -5703,8 +6049,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A82,$B$2)</f>
         <v>178</v>
       </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I82" cm="1">
+        <f t="array" ref="I82">iv($B$1,$B$2,G82,B82,C82,H82)</f>
+        <v>0.11478868846424191</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>172</v>
       </c>
@@ -5736,8 +6086,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A83,$B$2)</f>
         <v>148</v>
       </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I83" cm="1">
+        <f t="array" ref="I83">iv($B$1,$B$2,G83,B83,C83,H83)</f>
+        <v>0.11635428704553262</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>173</v>
       </c>
@@ -5769,8 +6123,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A84,$B$2)</f>
         <v>121</v>
       </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I84" cm="1">
+        <f t="array" ref="I84">iv($B$1,$B$2,G84,B84,C84,H84)</f>
+        <v>0.11712100606999017</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>174</v>
       </c>
@@ -5802,8 +6160,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A85,$B$2)</f>
         <v>98</v>
       </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I85" cm="1">
+        <f t="array" ref="I85">iv($B$1,$B$2,G85,B85,C85,H85)</f>
+        <v>0.11827144280411678</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>175</v>
       </c>
@@ -5835,8 +6197,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A86,$B$2)</f>
         <v>78</v>
       </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I86" cm="1">
+        <f t="array" ref="I86">iv($B$1,$B$2,G86,B86,C86,H86)</f>
+        <v>0.11889067961664918</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>176</v>
       </c>
@@ -5868,8 +6234,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A87,$B$2)</f>
         <v>61</v>
       </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I87" cm="1">
+        <f t="array" ref="I87">iv($B$1,$B$2,G87,B87,C87,H87)</f>
+        <v>0.11919627061552386</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>177</v>
       </c>
@@ -5901,8 +6271,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A88,$B$2)</f>
         <v>47.5</v>
       </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I88" cm="1">
+        <f t="array" ref="I88">iv($B$1,$B$2,G88,B88,C88,H88)</f>
+        <v>0.12011321325097986</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>178</v>
       </c>
@@ -5934,8 +6308,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A89,$B$2)</f>
         <v>36</v>
       </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I89" cm="1">
+        <f t="array" ref="I89">iv($B$1,$B$2,G89,B89,C89,H89)</f>
+        <v>0.12020321805512975</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>179</v>
       </c>
@@ -5967,8 +6345,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A90,$B$2)</f>
         <v>27</v>
       </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I90" cm="1">
+        <f t="array" ref="I90">iv($B$1,$B$2,G90,B90,C90,H90)</f>
+        <v>0.12051008143236905</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>180</v>
       </c>
@@ -6000,8 +6382,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A91,$B$2)</f>
         <v>20</v>
       </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I91" cm="1">
+        <f t="array" ref="I91">iv($B$1,$B$2,G91,B91,C91,H91)</f>
+        <v>0.12087011830912547</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>181</v>
       </c>
@@ -6033,8 +6419,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A92,$B$2)</f>
         <v>14.5</v>
       </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I92" cm="1">
+        <f t="array" ref="I92">iv($B$1,$B$2,G92,B92,C92,H92)</f>
+        <v>0.12095298543360126</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>182</v>
       </c>
@@ -6066,8 +6456,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A93,$B$2)</f>
         <v>10.5</v>
       </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I93" cm="1">
+        <f t="array" ref="I93">iv($B$1,$B$2,G93,B93,C93,H93)</f>
+        <v>0.12143756551855182</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>183</v>
       </c>
@@ -6099,8 +6493,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A94,$B$2)</f>
         <v>7.5</v>
       </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I94" cm="1">
+        <f t="array" ref="I94">iv($B$1,$B$2,G94,B94,C94,H94)</f>
+        <v>0.12185982440017973</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>184</v>
       </c>
@@ -6132,8 +6530,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A95,$B$2)</f>
         <v>5</v>
       </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I95" cm="1">
+        <f t="array" ref="I95">iv($B$1,$B$2,G95,B95,C95,H95)</f>
+        <v>0.1209482603374322</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>185</v>
       </c>
@@ -6165,8 +6567,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A96,$B$2)</f>
         <v>3.5</v>
       </c>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I96" cm="1">
+        <f t="array" ref="I96">iv($B$1,$B$2,G96,B96,C96,H96)</f>
+        <v>0.12153804261304957</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>186</v>
       </c>
@@ -6198,8 +6604,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A97,$B$2)</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I97" cm="1">
+        <f t="array" ref="I97">iv($B$1,$B$2,G97,B97,C97,H97)</f>
+        <v>0.11859513085413063</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>187</v>
       </c>
@@ -6231,8 +6641,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A98,$B$2)</f>
         <v>1.5</v>
       </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I98" cm="1">
+        <f t="array" ref="I98">iv($B$1,$B$2,G98,B98,C98,H98)</f>
+        <v>0.12088901555816914</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>188</v>
       </c>
@@ -6264,8 +6678,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A99,$B$2)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I99" cm="1">
+        <f t="array" ref="I99">iv($B$1,$B$2,G99,B99,C99,H99)</f>
+        <v>0.12125581745620084</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>189</v>
       </c>
@@ -6297,8 +6715,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A100,$B$2)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I100" cm="1">
+        <f t="array" ref="I100">iv($B$1,$B$2,G100,B100,C100,H100)</f>
+        <v>0.11786557077349274</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
         <v>190</v>
       </c>
@@ -6330,8 +6752,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A101,$B$2)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I101" cm="1">
+        <f t="array" ref="I101">iv($B$1,$B$2,G101,B101,C101,H101)</f>
+        <v>0.12393229883929972</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>191</v>
       </c>
@@ -6363,8 +6789,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A102,$B$2)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I102" cm="1">
+        <f t="array" ref="I102">iv($B$1,$B$2,G102,B102,C102,H102)</f>
+        <v>0.12990173805239666</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
         <v>192</v>
       </c>
@@ -6396,8 +6826,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A103,$B$2)</f>
         <v>626</v>
       </c>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I103" cm="1">
+        <f t="array" ref="I103">iv($B$1,$B$2,G103,B103,C103,H103)</f>
+        <v>6.4540404590849042E-14</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
         <v>193</v>
       </c>
@@ -6429,8 +6863,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A104,$B$2)</f>
         <v>533</v>
       </c>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I104" cm="1">
+        <f t="array" ref="I104">iv($B$1,$B$2,G104,B104,C104,H104)</f>
+        <v>1.2813118273880621E-14</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
         <v>194</v>
       </c>
@@ -6462,8 +6900,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A105,$B$2)</f>
         <v>445</v>
       </c>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I105" cm="1">
+        <f t="array" ref="I105">iv($B$1,$B$2,G105,B105,C105,H105)</f>
+        <v>9.1366957198216844E-2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
         <v>195</v>
       </c>
@@ -6495,8 +6937,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A106,$B$2)</f>
         <v>363</v>
       </c>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I106" cm="1">
+        <f t="array" ref="I106">iv($B$1,$B$2,G106,B106,C106,H106)</f>
+        <v>0.11288930581276597</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
         <v>196</v>
       </c>
@@ -6528,8 +6974,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A107,$B$2)</f>
         <v>289</v>
       </c>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I107" cm="1">
+        <f t="array" ref="I107">iv($B$1,$B$2,G107,B107,C107,H107)</f>
+        <v>0.12114582139113837</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
         <v>197</v>
       </c>
@@ -6561,8 +7011,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A108,$B$2)</f>
         <v>224.5</v>
       </c>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I108" cm="1">
+        <f t="array" ref="I108">iv($B$1,$B$2,G108,B108,C108,H108)</f>
+        <v>0.12605285458120241</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
         <v>198</v>
       </c>
@@ -6594,8 +7048,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A109,$B$2)</f>
         <v>169.5</v>
       </c>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I109" cm="1">
+        <f t="array" ref="I109">iv($B$1,$B$2,G109,B109,C109,H109)</f>
+        <v>0.128887448327692</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
         <v>199</v>
       </c>
@@ -6627,8 +7085,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A110,$B$2)</f>
         <v>124.5</v>
       </c>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I110" cm="1">
+        <f t="array" ref="I110">iv($B$1,$B$2,G110,B110,C110,H110)</f>
+        <v>0.13086418171506434</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
         <v>200</v>
       </c>
@@ -6660,8 +7122,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A111,$B$2)</f>
         <v>89</v>
       </c>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I111" cm="1">
+        <f t="array" ref="I111">iv($B$1,$B$2,G111,B111,C111,H111)</f>
+        <v>0.1323697351251126</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
         <v>201</v>
       </c>
@@ -6693,8 +7159,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A112,$B$2)</f>
         <v>61.5</v>
       </c>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I112" cm="1">
+        <f t="array" ref="I112">iv($B$1,$B$2,G112,B112,C112,H112)</f>
+        <v>0.13310731555485625</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
         <v>202</v>
       </c>
@@ -6726,8 +7196,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A113,$B$2)</f>
         <v>41.5</v>
       </c>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I113" cm="1">
+        <f t="array" ref="I113">iv($B$1,$B$2,G113,B113,C113,H113)</f>
+        <v>0.13394305027059633</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
         <v>203</v>
       </c>
@@ -6759,8 +7233,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A114,$B$2)</f>
         <v>27</v>
       </c>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I114" cm="1">
+        <f t="array" ref="I114">iv($B$1,$B$2,G114,B114,C114,H114)</f>
+        <v>0.13422498769371943</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
         <v>204</v>
       </c>
@@ -6792,8 +7270,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A115,$B$2)</f>
         <v>22</v>
       </c>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I115" cm="1">
+        <f t="array" ref="I115">iv($B$1,$B$2,G115,B115,C115,H115)</f>
+        <v>0.14382902952762608</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
         <v>205</v>
       </c>
@@ -6825,8 +7307,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A116,$B$2)</f>
         <v>603.5</v>
       </c>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I116" cm="1">
+        <f t="array" ref="I116">iv($B$1,$B$2,G116,B116,C116,H116)</f>
+        <v>2.4149748194128721E-13</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
         <v>206</v>
       </c>
@@ -6858,8 +7344,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A117,$B$2)</f>
         <v>515</v>
       </c>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I117" cm="1">
+        <f t="array" ref="I117">iv($B$1,$B$2,G117,B117,C117,H117)</f>
+        <v>5.3507797929809854E-13</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
         <v>207</v>
       </c>
@@ -6891,8 +7381,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A118,$B$2)</f>
         <v>433</v>
       </c>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I118" cm="1">
+        <f t="array" ref="I118">iv($B$1,$B$2,G118,B118,C118,H118)</f>
+        <v>0.10629619553572346</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
         <v>208</v>
       </c>
@@ -6924,8 +7418,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A119,$B$2)</f>
         <v>357</v>
       </c>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I119" cm="1">
+        <f t="array" ref="I119">iv($B$1,$B$2,G119,B119,C119,H119)</f>
+        <v>0.11624266264181789</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
         <v>209</v>
       </c>
@@ -6957,8 +7455,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A120,$B$2)</f>
         <v>289.5</v>
       </c>
-    </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I120" cm="1">
+        <f t="array" ref="I120">iv($B$1,$B$2,G120,B120,C120,H120)</f>
+        <v>0.12232724641629047</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
         <v>210</v>
       </c>
@@ -6990,8 +7492,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A121,$B$2)</f>
         <v>230</v>
       </c>
-    </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I121" cm="1">
+        <f t="array" ref="I121">iv($B$1,$B$2,G121,B121,C121,H121)</f>
+        <v>0.12590277200333749</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
         <v>211</v>
       </c>
@@ -7023,8 +7529,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A122,$B$2)</f>
         <v>179</v>
       </c>
-    </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I122" cm="1">
+        <f t="array" ref="I122">iv($B$1,$B$2,G122,B122,C122,H122)</f>
+        <v>0.12824557164413306</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
         <v>212</v>
       </c>
@@ -7056,8 +7566,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A123,$B$2)</f>
         <v>136.5</v>
       </c>
-    </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I123" cm="1">
+        <f t="array" ref="I123">iv($B$1,$B$2,G123,B123,C123,H123)</f>
+        <v>0.12991962872797364</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
         <v>213</v>
       </c>
@@ -7089,8 +7603,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A124,$B$2)</f>
         <v>102.5</v>
       </c>
-    </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I124" cm="1">
+        <f t="array" ref="I124">iv($B$1,$B$2,G124,B124,C124,H124)</f>
+        <v>0.13157041385441029</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A125" s="2" t="s">
         <v>214</v>
       </c>
@@ -7122,8 +7640,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A125,$B$2)</f>
         <v>75</v>
       </c>
-    </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I125" cm="1">
+        <f t="array" ref="I125">iv($B$1,$B$2,G125,B125,C125,H125)</f>
+        <v>0.1323939147636051</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A126" s="2" t="s">
         <v>215</v>
       </c>
@@ -7155,8 +7677,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A126,$B$2)</f>
         <v>54</v>
       </c>
-    </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I126" cm="1">
+        <f t="array" ref="I126">iv($B$1,$B$2,G126,B126,C126,H126)</f>
+        <v>0.13325449627308852</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
         <v>216</v>
       </c>
@@ -7188,8 +7714,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A127,$B$2)</f>
         <v>38</v>
       </c>
-    </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I127" cm="1">
+        <f t="array" ref="I127">iv($B$1,$B$2,G127,B127,C127,H127)</f>
+        <v>0.13376785025820653</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
         <v>217</v>
       </c>
@@ -7221,8 +7751,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A128,$B$2)</f>
         <v>531</v>
       </c>
-    </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I128" cm="1">
+        <f t="array" ref="I128">iv($B$1,$B$2,G128,B128,C128,H128)</f>
+        <v>7.4792304252037659E-2</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A129" s="2" t="s">
         <v>218</v>
       </c>
@@ -7254,8 +7788,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A129,$B$2)</f>
         <v>450.5</v>
       </c>
-    </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I129" cm="1">
+        <f t="array" ref="I129">iv($B$1,$B$2,G129,B129,C129,H129)</f>
+        <v>0.10406461861320009</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
         <v>219</v>
       </c>
@@ -7287,8 +7825,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A130,$B$2)</f>
         <v>377</v>
       </c>
-    </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I130" cm="1">
+        <f t="array" ref="I130">iv($B$1,$B$2,G130,B130,C130,H130)</f>
+        <v>0.11434444479430404</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">
         <v>220</v>
       </c>
@@ -7320,8 +7862,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A131,$B$2)</f>
         <v>310.5</v>
       </c>
-    </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I131" cm="1">
+        <f t="array" ref="I131">iv($B$1,$B$2,G131,B131,C131,H131)</f>
+        <v>0.12000109485235216</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
         <v>221</v>
       </c>
@@ -7353,8 +7899,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A132,$B$2)</f>
         <v>252</v>
       </c>
-    </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I132" cm="1">
+        <f t="array" ref="I132">iv($B$1,$B$2,G132,B132,C132,H132)</f>
+        <v>0.12389872564460182</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A133" s="2" t="s">
         <v>222</v>
       </c>
@@ -7386,8 +7936,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A133,$B$2)</f>
         <v>201</v>
       </c>
-    </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I133" cm="1">
+        <f t="array" ref="I133">iv($B$1,$B$2,G133,B133,C133,H133)</f>
+        <v>0.12640694740338107</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A134" s="2" t="s">
         <v>223</v>
       </c>
@@ -7419,8 +7973,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A134,$B$2)</f>
         <v>158</v>
       </c>
-    </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I134" cm="1">
+        <f t="array" ref="I134">iv($B$1,$B$2,G134,B134,C134,H134)</f>
+        <v>0.12842126577752302</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A135" s="2" t="s">
         <v>224</v>
       </c>
@@ -7452,8 +8010,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A135,$B$2)</f>
         <v>122</v>
       </c>
-    </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I135" cm="1">
+        <f t="array" ref="I135">iv($B$1,$B$2,G135,B135,C135,H135)</f>
+        <v>0.12977153942367975</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A136" s="2" t="s">
         <v>225</v>
       </c>
@@ -7485,8 +8047,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A136,$B$2)</f>
         <v>93</v>
       </c>
-    </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I136" cm="1">
+        <f t="array" ref="I136">iv($B$1,$B$2,G136,B136,C136,H136)</f>
+        <v>0.13104670814679859</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A137" s="2" t="s">
         <v>226</v>
       </c>
@@ -7518,8 +8084,12 @@
         <f>[1]!thsiFinD("ths_close_price_option",A137,$B$2)</f>
         <v>69.5</v>
       </c>
-    </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I137" cm="1">
+        <f t="array" ref="I137">iv($B$1,$B$2,G137,B137,C137,H137)</f>
+        <v>0.13178687764451189</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A138" s="2" t="s">
         <v>227</v>
       </c>
@@ -7550,6 +8120,10 @@
       <c r="H138" s="1">
         <f>[1]!thsiFinD("ths_close_price_option",A138,$B$2)</f>
         <v>51.5</v>
+      </c>
+      <c r="I138" cm="1">
+        <f t="array" ref="I138">iv($B$1,$B$2,G138,B138,C138,H138)</f>
+        <v>0.13273908262868703</v>
       </c>
     </row>
   </sheetData>
@@ -7560,7 +8134,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1"/>
   <sheetViews>
@@ -7568,7 +8142,7 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>